<commit_message>
Merge data in os itmes
</commit_message>
<xml_diff>
--- a/only_services.xlsx
+++ b/only_services.xlsx
@@ -1,15 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pixel-data-conversion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0ED25E-11C1-4B1B-BF23-22439DFBBA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Servicios" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1058,13 +1077,11 @@
   </si>
   <si>
     <t>SSD1TB - 1 - SSD SATA 2.5  1TB - 850.0
-SERV006 - 1 - Bateria OEM para Zbook - 197.41
 SERV006 - 1 - Bat He ZBook 15 G1 AR08 Negra 8C - 359
 ENVIOS - 1 - Envío - 72.5</t>
   </si>
   <si>
-    <t>SERV006 - 1 - Bateria OEM para DELL Precision 4500 49Wh - 197.41
-SERV006 - 1 - EKD6600  Bateria Li-ion 11.1V para Dell Precision M4600, M4700, M6600 - 365.4
+    <t>SERV006 - 1 - EKD6600  Bateria Li-ion 11.1V para Dell Precision M4600, M4700, M6600 - 365.4
 ENVIOS - 1 - Envío - 50.73</t>
   </si>
   <si>
@@ -1083,8 +1100,7 @@
 SERV 010 - 1 - Cargador Lenovo punta cuadrada 65w - 314.66</t>
   </si>
   <si>
-    <t>SERV006 - 1 - Bateria OEM para HP Pavilion 15-cw 11.4v 41Wh - 197.41
-SERV03 - 1 - Mantenimiento general - 250.0
+    <t>SERV03 - 1 - Mantenimiento general - 250.0
 SERV006 - 1 - XEKHHT03XL Bateria Interna (P) 11.4V para HP Pavilion 14-CE 14-CF 14-cm 14-CK 14-DF 14-MA 15-DA 15-CS 15-DB 14Q-CS 15-CW 17-by 17-CA HP 240 245 250 255 G7 340 348 G5 HT03XL - 324.8
 ENVIOS - 1 - Envío - 50.73</t>
   </si>
@@ -1115,8 +1131,7 @@
     <t>SERV006 - 1 - Bateria OEM para HP Pavilion 15-cw1xx 41Wh - 197.41</t>
   </si>
   <si>
-    <t>REF COMODÍN - 1 - Bateria OEM para Toshiba S55t-B 32Wh - 1270.2
-SERV006 - 1 - Bat To Sat L50-B PA5184U-1BRS Negra 4C - 229
+    <t>SERV006 - 1 - Bat To Sat L50-B PA5184U-1BRS Negra 4C - 229
 ENVIOS - 1 - Envío - 72.5</t>
   </si>
   <si>
@@ -1132,8 +1147,7 @@
     <t>SSDM.2NVME1TB - 1 - SSD M.2  NVME 1TB - 1412.93</t>
   </si>
   <si>
-    <t>REF COMODÍN - 1 - Teclado en Español para T430 Sin Retroiluminación - 1270.2
-REF COMODÍN - 1 - TEC387 Teclado color Negro (SP) para IBM Lenovo Thinkpad T530 X230 - 481.4
+    <t>REF COMODÍN - 1 - TEC387 Teclado color Negro (SP) para IBM Lenovo Thinkpad T530 X230 - 481.4
 ENVIOS - 1 - Envío - 7.25</t>
   </si>
   <si>
@@ -1156,15 +1170,13 @@
     <t>CADDYDISCO - 1 - Caddy para disco externo - 60.34</t>
   </si>
   <si>
-    <t>REF COMODÍN - 1 - Cargador Asus 65W - 1270.2
-REF COMODÍN - 1 - Cargador Asus Vivobook X441 X556 19v 3.42a 65w 4.0*1.35mm - 275</t>
+    <t>REF COMODÍN - 1 - Cargador Asus Vivobook X441 X556 19v 3.42a 65w 4.0*1.35mm - 275</t>
   </si>
   <si>
     <t>SERV 007 - 1 - Drenado de energía - 250.0</t>
   </si>
   <si>
-    <t>REF COMODÍN - 1 - Bateria OEM para DELL Inspiron E5570 62wh 7.6v 1 - 1270.2
-REF COMODÍN - 1 - EKD6MT4T Bateria Interna (P) 7.6V para Dell Latitude E5470/ E5570 Precision 3510 HK6DV 079VRK TXF9M 0TXF9M 6MT4T - 446.31
+    <t>REF COMODÍN - 1 - EKD6MT4T Bateria Interna (P) 7.6V para Dell Latitude E5470/ E5570 Precision 3510 HK6DV 079VRK TXF9M 0TXF9M 6MT4T - 446.31
 ENVIOS - 1 - Envío - 68.09</t>
   </si>
   <si>
@@ -1188,8 +1200,7 @@
 SERV03 - 1 - Mantenimiento general - 250.0</t>
   </si>
   <si>
-    <t>REF COMODÍN - 1 - Bateria OEM para DELL Inspiron 15  7000 11.1v 43Wh - 1270.2
-REF COMODÍN - 1 - EKDGK5KY Bateria 11.4V 43Wh para Dell Inspiron 11 3000 series / 13 7000 series / 15 7000 GK5KY - 440.8
+    <t>REF COMODÍN - 1 - EKDGK5KY Bateria 11.4V 43Wh para Dell Inspiron 11 3000 series / 13 7000 series / 15 7000 GK5KY - 440.8
 ENVIOS - 1 - Envío - 68.09</t>
   </si>
   <si>
@@ -1204,12 +1215,7 @@
     <t>Gar002 - 1 - Garantia Centro de Servicio - 0.0</t>
   </si>
   <si>
-    <t>REF COMODÍN - 1 - Teclado par Lenovo T570 en Español No
-retroiluminado - 1270.2
-REF COMODÍN - 1 - Teclado para Lenovo T460 en Español No
-retroiluminado - 1270.2
-REF COMODÍN - 1 - Display 14" LED 1366x768 Bisel Delgado - 1270.2
-REF COMODÍN - 1 - TEC491 Teclado color Negro (SP) para Lenovo E431 T440 L440 E440 T450 T460 - 336.4
+    <t>REF COMODÍN - 1 - TEC491 Teclado color Negro (SP) para Lenovo E431 T440 L440 E440 T450 T460 - 336.4
 REF COMODÍN - 1 - TEC526 Teclado color Negro (SP) para Lenovo E531 E540 L540 L570 T540 T550 W540 W550s Series - 452.4
 REF COMODÍN - 1 - LCD140-015D Pantalla LCD 14.0 LED WXGA (1366X768) Slim Conector Inferior Derecho 30P Glossy 315mm (bezel delgado) - 696
 ENVIOS - 1 - Envío - 20.66</t>
@@ -1219,7 +1225,6 @@
   </si>
   <si>
     <t>SSD256 - 1 - SSD SATA 2.5  256GB - 650.86
-REF COMODÍN - 1 - Bateria OEM para Acer Aspire A523 14.6v 32Wh - 1270.2
 REF COMODÍN - 1 - Bateria para ACER BT12122 - 245</t>
   </si>
   <si>
@@ -1684,11 +1689,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1755,13 +1760,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1799,7 +1812,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1833,6 +1846,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1867,9 +1881,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2042,17 +2057,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K134"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F135" sqref="F135"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="70.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="88.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2087,7 +2105,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2095,7 +2113,7 @@
         <v>144</v>
       </c>
       <c r="C2" s="3">
-        <v>45293.40916666666</v>
+        <v>45293.409166666657</v>
       </c>
       <c r="D2" t="s">
         <v>247</v>
@@ -2119,7 +2137,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2127,7 +2145,7 @@
         <v>145</v>
       </c>
       <c r="C3" s="3">
-        <v>45293.42548611111</v>
+        <v>45293.425486111111</v>
       </c>
       <c r="D3" t="s">
         <v>248</v>
@@ -2151,7 +2169,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -2159,7 +2177,7 @@
         <v>146</v>
       </c>
       <c r="C4" s="3">
-        <v>45293.43032407408</v>
+        <v>45293.430324074077</v>
       </c>
       <c r="D4" t="s">
         <v>249</v>
@@ -2168,7 +2186,7 @@
         <v>347</v>
       </c>
       <c r="F4">
-        <v>1478.91</v>
+        <v>1281.5</v>
       </c>
       <c r="G4">
         <v>3424</v>
@@ -2186,7 +2204,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2194,7 +2212,7 @@
         <v>147</v>
       </c>
       <c r="C5" s="3">
-        <v>45293.43159722222</v>
+        <v>45293.431597222218</v>
       </c>
       <c r="D5" t="s">
         <v>250</v>
@@ -2203,7 +2221,7 @@
         <v>348</v>
       </c>
       <c r="F5">
-        <v>613.54</v>
+        <v>416.13</v>
       </c>
       <c r="G5">
         <v>1972</v>
@@ -2221,7 +2239,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -2229,7 +2247,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="3">
-        <v>45293.49710648148</v>
+        <v>45293.497106481482</v>
       </c>
       <c r="D6" t="s">
         <v>251</v>
@@ -2253,7 +2271,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2261,7 +2279,7 @@
         <v>149</v>
       </c>
       <c r="C7" s="3">
-        <v>45293.520625</v>
+        <v>45293.520624999997</v>
       </c>
       <c r="D7" t="s">
         <v>252</v>
@@ -2285,7 +2303,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -2293,7 +2311,7 @@
         <v>150</v>
       </c>
       <c r="C8" s="3">
-        <v>45293.5405787037</v>
+        <v>45293.540578703702</v>
       </c>
       <c r="D8" t="s">
         <v>253</v>
@@ -2317,7 +2335,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -2325,7 +2343,7 @@
         <v>151</v>
       </c>
       <c r="C9" s="3">
-        <v>45293.63739583334</v>
+        <v>45293.637395833342</v>
       </c>
       <c r="D9" t="s">
         <v>254</v>
@@ -2346,7 +2364,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2354,7 +2372,7 @@
         <v>151</v>
       </c>
       <c r="C10" s="3">
-        <v>45293.64356481482</v>
+        <v>45293.643564814818</v>
       </c>
       <c r="D10" t="s">
         <v>254</v>
@@ -2363,7 +2381,7 @@
         <v>353</v>
       </c>
       <c r="F10">
-        <v>822.9400000000001</v>
+        <v>625.53</v>
       </c>
       <c r="G10">
         <v>2436</v>
@@ -2381,7 +2399,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2389,7 +2407,7 @@
         <v>152</v>
       </c>
       <c r="C11" s="3">
-        <v>45293.64849537037</v>
+        <v>45293.648495370369</v>
       </c>
       <c r="D11" t="s">
         <v>255</v>
@@ -2413,7 +2431,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -2421,7 +2439,7 @@
         <v>153</v>
       </c>
       <c r="C12" s="3">
-        <v>45293.69689814815</v>
+        <v>45293.696898148148</v>
       </c>
       <c r="D12" t="s">
         <v>256</v>
@@ -2442,7 +2460,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2450,7 +2468,7 @@
         <v>154</v>
       </c>
       <c r="C13" s="3">
-        <v>45293.72875</v>
+        <v>45293.728750000002</v>
       </c>
       <c r="D13" t="s">
         <v>257</v>
@@ -2474,7 +2492,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -2482,7 +2500,7 @@
         <v>155</v>
       </c>
       <c r="C14" s="3">
-        <v>45293.73319444444</v>
+        <v>45293.733194444438</v>
       </c>
       <c r="D14" t="s">
         <v>258</v>
@@ -2503,7 +2521,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -2511,7 +2529,7 @@
         <v>156</v>
       </c>
       <c r="C15" s="3">
-        <v>45293.73402777778</v>
+        <v>45293.734027777777</v>
       </c>
       <c r="D15" t="s">
         <v>259</v>
@@ -2535,7 +2553,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -2567,7 +2585,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -2575,7 +2593,7 @@
         <v>158</v>
       </c>
       <c r="C17" s="3">
-        <v>45294.52268518518</v>
+        <v>45294.522685185177</v>
       </c>
       <c r="D17" t="s">
         <v>261</v>
@@ -2599,7 +2617,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -2607,7 +2625,7 @@
         <v>159</v>
       </c>
       <c r="C18" s="3">
-        <v>45294.69050925926</v>
+        <v>45294.690509259257</v>
       </c>
       <c r="D18" t="s">
         <v>262</v>
@@ -2631,7 +2649,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -2639,7 +2657,7 @@
         <v>160</v>
       </c>
       <c r="C19" s="3">
-        <v>45295.41672453703</v>
+        <v>45295.416724537034</v>
       </c>
       <c r="D19" t="s">
         <v>263</v>
@@ -2663,7 +2681,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -2671,7 +2689,7 @@
         <v>161</v>
       </c>
       <c r="C20" s="3">
-        <v>45295.50078703704</v>
+        <v>45295.500787037039</v>
       </c>
       <c r="D20" t="s">
         <v>264</v>
@@ -2695,7 +2713,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -2703,7 +2721,7 @@
         <v>162</v>
       </c>
       <c r="C21" s="3">
-        <v>45295.5046412037</v>
+        <v>45295.504641203697</v>
       </c>
       <c r="D21" t="s">
         <v>265</v>
@@ -2727,7 +2745,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -2735,7 +2753,7 @@
         <v>163</v>
       </c>
       <c r="C22" s="3">
-        <v>45295.56520833333</v>
+        <v>45295.565208333333</v>
       </c>
       <c r="D22" t="s">
         <v>266</v>
@@ -2759,7 +2777,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -2767,7 +2785,7 @@
         <v>164</v>
       </c>
       <c r="C23" s="3">
-        <v>45295.59929398148</v>
+        <v>45295.599293981482</v>
       </c>
       <c r="D23" t="s">
         <v>267</v>
@@ -2788,7 +2806,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -2796,7 +2814,7 @@
         <v>165</v>
       </c>
       <c r="C24" s="3">
-        <v>45295.60870370371</v>
+        <v>45295.608703703707</v>
       </c>
       <c r="D24" t="s">
         <v>268</v>
@@ -2820,7 +2838,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -2828,7 +2846,7 @@
         <v>166</v>
       </c>
       <c r="C25" s="3">
-        <v>45295.71038194445</v>
+        <v>45295.710381944453</v>
       </c>
       <c r="D25" t="s">
         <v>269</v>
@@ -2852,7 +2870,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -2860,7 +2878,7 @@
         <v>166</v>
       </c>
       <c r="C26" s="3">
-        <v>45295.71620370371</v>
+        <v>45295.716203703712</v>
       </c>
       <c r="D26" t="s">
         <v>269</v>
@@ -2884,7 +2902,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -2892,7 +2910,7 @@
         <v>167</v>
       </c>
       <c r="C27" s="3">
-        <v>45295.75900462963</v>
+        <v>45295.759004629632</v>
       </c>
       <c r="D27" t="s">
         <v>270</v>
@@ -2916,7 +2934,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -2924,7 +2942,7 @@
         <v>168</v>
       </c>
       <c r="C28" s="3">
-        <v>45296.48380787037</v>
+        <v>45296.483807870369</v>
       </c>
       <c r="D28" t="s">
         <v>271</v>
@@ -2933,7 +2951,7 @@
         <v>362</v>
       </c>
       <c r="F28">
-        <v>1571.7</v>
+        <v>301.5</v>
       </c>
       <c r="G28">
         <v>1624</v>
@@ -2951,7 +2969,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -2959,7 +2977,7 @@
         <v>169</v>
       </c>
       <c r="C29" s="3">
-        <v>45296.70635416666</v>
+        <v>45296.706354166658</v>
       </c>
       <c r="D29" t="s">
         <v>272</v>
@@ -2983,7 +3001,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -3015,7 +3033,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -3023,7 +3041,7 @@
         <v>169</v>
       </c>
       <c r="C31" s="3">
-        <v>45296.71063657408</v>
+        <v>45296.710636574076</v>
       </c>
       <c r="D31" t="s">
         <v>272</v>
@@ -3047,7 +3065,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -3055,7 +3073,7 @@
         <v>169</v>
       </c>
       <c r="C32" s="3">
-        <v>45296.71376157407</v>
+        <v>45296.713761574072</v>
       </c>
       <c r="D32" t="s">
         <v>272</v>
@@ -3079,7 +3097,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -3111,7 +3129,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -3119,7 +3137,7 @@
         <v>170</v>
       </c>
       <c r="C34" s="3">
-        <v>45296.7368287037</v>
+        <v>45296.736828703702</v>
       </c>
       <c r="D34" t="s">
         <v>273</v>
@@ -3143,7 +3161,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -3175,7 +3193,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -3183,7 +3201,7 @@
         <v>172</v>
       </c>
       <c r="C36" s="3">
-        <v>45297.44438657408</v>
+        <v>45297.444386574083</v>
       </c>
       <c r="D36" t="s">
         <v>275</v>
@@ -3207,7 +3225,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -3215,7 +3233,7 @@
         <v>173</v>
       </c>
       <c r="C37" s="3">
-        <v>45299.65844907407</v>
+        <v>45299.658449074072</v>
       </c>
       <c r="D37" t="s">
         <v>276</v>
@@ -3239,7 +3257,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -3271,7 +3289,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -3279,7 +3297,7 @@
         <v>175</v>
       </c>
       <c r="C39" s="3">
-        <v>45299.7290162037</v>
+        <v>45299.729016203702</v>
       </c>
       <c r="D39" t="s">
         <v>278</v>
@@ -3303,7 +3321,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -3311,7 +3329,7 @@
         <v>176</v>
       </c>
       <c r="C40" s="3">
-        <v>45299.76886574074</v>
+        <v>45299.768865740742</v>
       </c>
       <c r="D40" t="s">
         <v>279</v>
@@ -3335,7 +3353,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>50</v>
       </c>
@@ -3352,7 +3370,7 @@
         <v>367</v>
       </c>
       <c r="F41">
-        <v>1758.85</v>
+        <v>488.65</v>
       </c>
       <c r="G41">
         <v>1400</v>
@@ -3370,7 +3388,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>51</v>
       </c>
@@ -3378,7 +3396,7 @@
         <v>178</v>
       </c>
       <c r="C42" s="3">
-        <v>45300.6213425926</v>
+        <v>45300.621342592603</v>
       </c>
       <c r="D42" t="s">
         <v>281</v>
@@ -3402,7 +3420,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -3410,7 +3428,7 @@
         <v>179</v>
       </c>
       <c r="C43" s="3">
-        <v>45300.63311342592</v>
+        <v>45300.633113425924</v>
       </c>
       <c r="D43" t="s">
         <v>282</v>
@@ -3419,7 +3437,7 @@
         <v>368</v>
       </c>
       <c r="F43">
-        <v>512.0700000000001</v>
+        <v>512.07000000000005</v>
       </c>
       <c r="G43">
         <v>2900</v>
@@ -3434,7 +3452,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -3442,7 +3460,7 @@
         <v>180</v>
       </c>
       <c r="C44" s="3">
-        <v>45300.675</v>
+        <v>45300.675000000003</v>
       </c>
       <c r="D44" t="s">
         <v>283</v>
@@ -3466,7 +3484,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -3474,7 +3492,7 @@
         <v>164</v>
       </c>
       <c r="C45" s="3">
-        <v>45300.69486111111</v>
+        <v>45300.694861111107</v>
       </c>
       <c r="D45" t="s">
         <v>267</v>
@@ -3498,7 +3516,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -3506,7 +3524,7 @@
         <v>181</v>
       </c>
       <c r="C46" s="3">
-        <v>45300.73149305556</v>
+        <v>45300.731493055559</v>
       </c>
       <c r="D46" t="s">
         <v>284</v>
@@ -3530,7 +3548,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>56</v>
       </c>
@@ -3538,7 +3556,7 @@
         <v>182</v>
       </c>
       <c r="C47" s="3">
-        <v>45301.38350694445</v>
+        <v>45301.383506944447</v>
       </c>
       <c r="D47" t="s">
         <v>285</v>
@@ -3565,7 +3583,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>57</v>
       </c>
@@ -3573,7 +3591,7 @@
         <v>183</v>
       </c>
       <c r="C48" s="3">
-        <v>45301.45447916666</v>
+        <v>45301.454479166663</v>
       </c>
       <c r="D48" t="s">
         <v>286</v>
@@ -3597,7 +3615,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>58</v>
       </c>
@@ -3605,7 +3623,7 @@
         <v>184</v>
       </c>
       <c r="C49" s="3">
-        <v>45301.56194444445</v>
+        <v>45301.561944444453</v>
       </c>
       <c r="D49" t="s">
         <v>287</v>
@@ -3629,7 +3647,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>59</v>
       </c>
@@ -3637,7 +3655,7 @@
         <v>185</v>
       </c>
       <c r="C50" s="3">
-        <v>45301.5903125</v>
+        <v>45301.590312499997</v>
       </c>
       <c r="D50" t="s">
         <v>288</v>
@@ -3661,7 +3679,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>60</v>
       </c>
@@ -3669,7 +3687,7 @@
         <v>186</v>
       </c>
       <c r="C51" s="3">
-        <v>45301.64981481482</v>
+        <v>45301.649814814817</v>
       </c>
       <c r="D51" t="s">
         <v>289</v>
@@ -3693,7 +3711,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>61</v>
       </c>
@@ -3701,7 +3719,7 @@
         <v>187</v>
       </c>
       <c r="C52" s="3">
-        <v>45301.70329861111</v>
+        <v>45301.703298611108</v>
       </c>
       <c r="D52" t="s">
         <v>290</v>
@@ -3725,7 +3743,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>62</v>
       </c>
@@ -3733,7 +3751,7 @@
         <v>188</v>
       </c>
       <c r="C53" s="3">
-        <v>45301.72096064815</v>
+        <v>45301.720960648148</v>
       </c>
       <c r="D53" t="s">
         <v>291</v>
@@ -3757,7 +3775,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>63</v>
       </c>
@@ -3765,7 +3783,7 @@
         <v>174</v>
       </c>
       <c r="C54" s="3">
-        <v>45301.76365740741</v>
+        <v>45301.763657407413</v>
       </c>
       <c r="D54" t="s">
         <v>292</v>
@@ -3774,7 +3792,7 @@
         <v>371</v>
       </c>
       <c r="F54">
-        <v>314.66</v>
+        <v>314.66000000000003</v>
       </c>
       <c r="G54">
         <v>1150</v>
@@ -3786,7 +3804,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -3794,7 +3812,7 @@
         <v>189</v>
       </c>
       <c r="C55" s="3">
-        <v>45302.43177083333</v>
+        <v>45302.431770833333</v>
       </c>
       <c r="D55" t="s">
         <v>293</v>
@@ -3815,7 +3833,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>65</v>
       </c>
@@ -3823,7 +3841,7 @@
         <v>190</v>
       </c>
       <c r="C56" s="3">
-        <v>45302.57895833333</v>
+        <v>45302.578958333332</v>
       </c>
       <c r="D56" t="s">
         <v>294</v>
@@ -3847,7 +3865,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>66</v>
       </c>
@@ -3855,7 +3873,7 @@
         <v>191</v>
       </c>
       <c r="C57" s="3">
-        <v>45302.66740740741</v>
+        <v>45302.667407407411</v>
       </c>
       <c r="D57" t="s">
         <v>295</v>
@@ -3876,7 +3894,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>67</v>
       </c>
@@ -3884,7 +3902,7 @@
         <v>192</v>
       </c>
       <c r="C58" s="3">
-        <v>45303.54585648148</v>
+        <v>45303.545856481483</v>
       </c>
       <c r="D58" t="s">
         <v>296</v>
@@ -3908,7 +3926,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>68</v>
       </c>
@@ -3916,7 +3934,7 @@
         <v>193</v>
       </c>
       <c r="C59" s="3">
-        <v>45303.74936342592</v>
+        <v>45303.749363425923</v>
       </c>
       <c r="D59" t="s">
         <v>297</v>
@@ -3940,7 +3958,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>69</v>
       </c>
@@ -3948,7 +3966,7 @@
         <v>194</v>
       </c>
       <c r="C60" s="3">
-        <v>45304.43210648148</v>
+        <v>45304.432106481479</v>
       </c>
       <c r="D60" t="s">
         <v>298</v>
@@ -3957,7 +3975,7 @@
         <v>374</v>
       </c>
       <c r="F60">
-        <v>1545.2</v>
+        <v>275</v>
       </c>
       <c r="G60">
         <v>650</v>
@@ -3972,7 +3990,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -3980,7 +3998,7 @@
         <v>195</v>
       </c>
       <c r="C61" s="3">
-        <v>45304.52567129629</v>
+        <v>45304.525671296287</v>
       </c>
       <c r="D61" t="s">
         <v>299</v>
@@ -4004,7 +4022,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>71</v>
       </c>
@@ -4012,7 +4030,7 @@
         <v>196</v>
       </c>
       <c r="C62" s="3">
-        <v>45306.48765046296</v>
+        <v>45306.487650462957</v>
       </c>
       <c r="D62" t="s">
         <v>300</v>
@@ -4036,7 +4054,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>72</v>
       </c>
@@ -4044,7 +4062,7 @@
         <v>197</v>
       </c>
       <c r="C63" s="3">
-        <v>45306.49606481481</v>
+        <v>45306.496064814812</v>
       </c>
       <c r="D63" t="s">
         <v>288</v>
@@ -4053,7 +4071,7 @@
         <v>376</v>
       </c>
       <c r="F63">
-        <v>1784.6</v>
+        <v>514.4</v>
       </c>
       <c r="G63">
         <v>1600</v>
@@ -4071,7 +4089,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>73</v>
       </c>
@@ -4079,7 +4097,7 @@
         <v>198</v>
       </c>
       <c r="C64" s="3">
-        <v>45306.51649305555</v>
+        <v>45306.516493055547</v>
       </c>
       <c r="D64" t="s">
         <v>301</v>
@@ -4103,7 +4121,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>74</v>
       </c>
@@ -4111,7 +4129,7 @@
         <v>198</v>
       </c>
       <c r="C65" s="3">
-        <v>45306.52288194445</v>
+        <v>45306.522881944453</v>
       </c>
       <c r="D65" t="s">
         <v>301</v>
@@ -4135,7 +4153,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>75</v>
       </c>
@@ -4143,7 +4161,7 @@
         <v>198</v>
       </c>
       <c r="C66" s="3">
-        <v>45306.5281712963</v>
+        <v>45306.528171296297</v>
       </c>
       <c r="D66" t="s">
         <v>301</v>
@@ -4167,7 +4185,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>76</v>
       </c>
@@ -4175,7 +4193,7 @@
         <v>199</v>
       </c>
       <c r="C67" s="3">
-        <v>45306.5890625</v>
+        <v>45306.589062500003</v>
       </c>
       <c r="D67" t="s">
         <v>302</v>
@@ -4199,7 +4217,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>77</v>
       </c>
@@ -4207,7 +4225,7 @@
         <v>200</v>
       </c>
       <c r="C68" s="3">
-        <v>45306.69413194444</v>
+        <v>45306.694131944438</v>
       </c>
       <c r="D68" t="s">
         <v>303</v>
@@ -4231,7 +4249,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>78</v>
       </c>
@@ -4239,7 +4257,7 @@
         <v>172</v>
       </c>
       <c r="C69" s="3">
-        <v>45307.50402777778</v>
+        <v>45307.504027777781</v>
       </c>
       <c r="D69" t="s">
         <v>275</v>
@@ -4263,7 +4281,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>79</v>
       </c>
@@ -4271,7 +4289,7 @@
         <v>201</v>
       </c>
       <c r="C70" s="3">
-        <v>45307.50483796297</v>
+        <v>45307.504837962973</v>
       </c>
       <c r="D70" t="s">
         <v>304</v>
@@ -4295,7 +4313,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>80</v>
       </c>
@@ -4303,7 +4321,7 @@
         <v>202</v>
       </c>
       <c r="C71" s="3">
-        <v>45307.5415162037</v>
+        <v>45307.541516203702</v>
       </c>
       <c r="D71" t="s">
         <v>305</v>
@@ -4327,7 +4345,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>81</v>
       </c>
@@ -4335,7 +4353,7 @@
         <v>203</v>
       </c>
       <c r="C72" s="3">
-        <v>45307.54159722223</v>
+        <v>45307.541597222233</v>
       </c>
       <c r="D72" t="s">
         <v>288</v>
@@ -4356,7 +4374,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>82</v>
       </c>
@@ -4364,7 +4382,7 @@
         <v>169</v>
       </c>
       <c r="C73" s="3">
-        <v>45307.69207175926</v>
+        <v>45307.692071759258</v>
       </c>
       <c r="D73" t="s">
         <v>272</v>
@@ -4388,7 +4406,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>83</v>
       </c>
@@ -4396,7 +4414,7 @@
         <v>169</v>
       </c>
       <c r="C74" s="3">
-        <v>45307.69337962963</v>
+        <v>45307.693379629629</v>
       </c>
       <c r="D74" t="s">
         <v>272</v>
@@ -4420,7 +4438,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>84</v>
       </c>
@@ -4428,7 +4446,7 @@
         <v>204</v>
       </c>
       <c r="C75" s="3">
-        <v>45307.72324074074</v>
+        <v>45307.723240740743</v>
       </c>
       <c r="D75" t="s">
         <v>306</v>
@@ -4452,7 +4470,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>85</v>
       </c>
@@ -4460,7 +4478,7 @@
         <v>183</v>
       </c>
       <c r="C76" s="3">
-        <v>45307.74225694445</v>
+        <v>45307.742256944453</v>
       </c>
       <c r="D76" t="s">
         <v>286</v>
@@ -4484,7 +4502,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>86</v>
       </c>
@@ -4492,7 +4510,7 @@
         <v>205</v>
       </c>
       <c r="C77" s="3">
-        <v>45308.72087962963</v>
+        <v>45308.720879629633</v>
       </c>
       <c r="D77" t="s">
         <v>307</v>
@@ -4513,7 +4531,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>87</v>
       </c>
@@ -4521,7 +4539,7 @@
         <v>206</v>
       </c>
       <c r="C78" s="3">
-        <v>45308.72868055556</v>
+        <v>45308.728680555563</v>
       </c>
       <c r="D78" t="s">
         <v>308</v>
@@ -4545,7 +4563,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>88</v>
       </c>
@@ -4553,7 +4571,7 @@
         <v>206</v>
       </c>
       <c r="C79" s="3">
-        <v>45308.73480324074</v>
+        <v>45308.734803240739</v>
       </c>
       <c r="D79" t="s">
         <v>308</v>
@@ -4577,7 +4595,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>89</v>
       </c>
@@ -4585,7 +4603,7 @@
         <v>174</v>
       </c>
       <c r="C80" s="3">
-        <v>45308.74643518519</v>
+        <v>45308.746435185189</v>
       </c>
       <c r="D80" t="s">
         <v>309</v>
@@ -4609,7 +4627,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>90</v>
       </c>
@@ -4617,7 +4635,7 @@
         <v>207</v>
       </c>
       <c r="C81" s="3">
-        <v>45309.39240740741</v>
+        <v>45309.392407407409</v>
       </c>
       <c r="D81" t="s">
         <v>310</v>
@@ -4641,7 +4659,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>91</v>
       </c>
@@ -4649,7 +4667,7 @@
         <v>208</v>
       </c>
       <c r="C82" s="3">
-        <v>45309.53040509259</v>
+        <v>45309.530405092592</v>
       </c>
       <c r="D82" t="s">
         <v>311</v>
@@ -4658,7 +4676,7 @@
         <v>383</v>
       </c>
       <c r="F82">
-        <v>1779.09</v>
+        <v>508.89</v>
       </c>
       <c r="G82">
         <v>1600</v>
@@ -4676,7 +4694,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>92</v>
       </c>
@@ -4708,7 +4726,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>93</v>
       </c>
@@ -4716,7 +4734,7 @@
         <v>210</v>
       </c>
       <c r="C84" s="3">
-        <v>45309.72028935186</v>
+        <v>45309.720289351862</v>
       </c>
       <c r="D84" t="s">
         <v>313</v>
@@ -4740,7 +4758,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>94</v>
       </c>
@@ -4748,7 +4766,7 @@
         <v>211</v>
       </c>
       <c r="C85" s="3">
-        <v>45310.48010416667</v>
+        <v>45310.480104166672</v>
       </c>
       <c r="D85" t="s">
         <v>314</v>
@@ -4772,7 +4790,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>95</v>
       </c>
@@ -4780,7 +4798,7 @@
         <v>212</v>
       </c>
       <c r="C86" s="3">
-        <v>45310.60517361111</v>
+        <v>45310.605173611111</v>
       </c>
       <c r="D86" t="s">
         <v>315</v>
@@ -4804,7 +4822,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>96</v>
       </c>
@@ -4812,7 +4830,7 @@
         <v>213</v>
       </c>
       <c r="C87" s="3">
-        <v>45310.74252314815</v>
+        <v>45310.742523148147</v>
       </c>
       <c r="D87" t="s">
         <v>316</v>
@@ -4836,7 +4854,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>97</v>
       </c>
@@ -4844,7 +4862,7 @@
         <v>162</v>
       </c>
       <c r="C88" s="3">
-        <v>45311.50221064815</v>
+        <v>45311.502210648148</v>
       </c>
       <c r="D88" t="s">
         <v>265</v>
@@ -4868,7 +4886,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>98</v>
       </c>
@@ -4876,7 +4894,7 @@
         <v>214</v>
       </c>
       <c r="C89" s="3">
-        <v>45313.39831018518</v>
+        <v>45313.398310185177</v>
       </c>
       <c r="D89" t="s">
         <v>317</v>
@@ -4900,7 +4918,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>99</v>
       </c>
@@ -4908,7 +4926,7 @@
         <v>215</v>
       </c>
       <c r="C90" s="3">
-        <v>45313.46736111111</v>
+        <v>45313.467361111107</v>
       </c>
       <c r="D90" t="s">
         <v>318</v>
@@ -4932,7 +4950,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>100</v>
       </c>
@@ -4940,7 +4958,7 @@
         <v>215</v>
       </c>
       <c r="C91" s="3">
-        <v>45313.47009259259</v>
+        <v>45313.470092592594</v>
       </c>
       <c r="D91" t="s">
         <v>318</v>
@@ -4964,7 +4982,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>101</v>
       </c>
@@ -4972,7 +4990,7 @@
         <v>216</v>
       </c>
       <c r="C92" s="3">
-        <v>45313.50326388889</v>
+        <v>45313.503263888888</v>
       </c>
       <c r="D92" t="s">
         <v>288</v>
@@ -4981,7 +4999,7 @@
         <v>387</v>
       </c>
       <c r="F92">
-        <v>5316.06</v>
+        <v>1505.46</v>
       </c>
       <c r="G92">
         <v>4200</v>
@@ -4996,7 +5014,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>102</v>
       </c>
@@ -5004,7 +5022,7 @@
         <v>174</v>
       </c>
       <c r="C93" s="3">
-        <v>45313.54563657408</v>
+        <v>45313.545636574083</v>
       </c>
       <c r="D93" t="s">
         <v>288</v>
@@ -5028,7 +5046,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="94" spans="1:11">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>103</v>
       </c>
@@ -5036,7 +5054,7 @@
         <v>185</v>
       </c>
       <c r="C94" s="3">
-        <v>45313.69777777778</v>
+        <v>45313.697777777779</v>
       </c>
       <c r="D94" t="s">
         <v>288</v>
@@ -5060,7 +5078,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="95" spans="1:11">
+    <row r="95" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>104</v>
       </c>
@@ -5068,7 +5086,7 @@
         <v>217</v>
       </c>
       <c r="C95" s="3">
-        <v>45314.38986111111</v>
+        <v>45314.389861111107</v>
       </c>
       <c r="D95" t="s">
         <v>319</v>
@@ -5077,7 +5095,7 @@
         <v>389</v>
       </c>
       <c r="F95">
-        <v>2166.06</v>
+        <v>895.86</v>
       </c>
       <c r="G95">
         <v>3500</v>
@@ -5095,7 +5113,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="96" spans="1:11">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>105</v>
       </c>
@@ -5103,7 +5121,7 @@
         <v>218</v>
       </c>
       <c r="C96" s="3">
-        <v>45314.4425462963</v>
+        <v>45314.442546296297</v>
       </c>
       <c r="D96" t="s">
         <v>320</v>
@@ -5127,7 +5145,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="97" spans="1:11">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>106</v>
       </c>
@@ -5135,7 +5153,7 @@
         <v>219</v>
       </c>
       <c r="C97" s="3">
-        <v>45314.49410879629</v>
+        <v>45314.494108796287</v>
       </c>
       <c r="D97" t="s">
         <v>321</v>
@@ -5159,7 +5177,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="98" spans="1:11">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>107</v>
       </c>
@@ -5167,7 +5185,7 @@
         <v>220</v>
       </c>
       <c r="C98" s="3">
-        <v>45314.51045138889</v>
+        <v>45314.510451388887</v>
       </c>
       <c r="D98" t="s">
         <v>322</v>
@@ -5191,7 +5209,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>108</v>
       </c>
@@ -5223,7 +5241,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>109</v>
       </c>
@@ -5231,7 +5249,7 @@
         <v>174</v>
       </c>
       <c r="C100" s="3">
-        <v>45314.5341550926</v>
+        <v>45314.534155092602</v>
       </c>
       <c r="D100" t="s">
         <v>292</v>
@@ -5252,7 +5270,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>110</v>
       </c>
@@ -5260,7 +5278,7 @@
         <v>222</v>
       </c>
       <c r="C101" s="3">
-        <v>45314.54357638889</v>
+        <v>45314.543576388889</v>
       </c>
       <c r="D101" t="s">
         <v>324</v>
@@ -5284,7 +5302,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="102" spans="1:11">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>111</v>
       </c>
@@ -5292,7 +5310,7 @@
         <v>223</v>
       </c>
       <c r="C102" s="3">
-        <v>45314.54976851852</v>
+        <v>45314.549768518518</v>
       </c>
       <c r="D102" t="s">
         <v>325</v>
@@ -5316,7 +5334,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="103" spans="1:11">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>112</v>
       </c>
@@ -5324,7 +5342,7 @@
         <v>224</v>
       </c>
       <c r="C103" s="3">
-        <v>45314.55601851852</v>
+        <v>45314.556018518517</v>
       </c>
       <c r="D103" t="s">
         <v>326</v>
@@ -5348,7 +5366,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="104" spans="1:11">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>113</v>
       </c>
@@ -5356,7 +5374,7 @@
         <v>224</v>
       </c>
       <c r="C104" s="3">
-        <v>45314.56140046296</v>
+        <v>45314.561400462961</v>
       </c>
       <c r="D104" t="s">
         <v>326</v>
@@ -5380,7 +5398,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="105" spans="1:11">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>114</v>
       </c>
@@ -5388,7 +5406,7 @@
         <v>225</v>
       </c>
       <c r="C105" s="3">
-        <v>45314.58067129629</v>
+        <v>45314.580671296288</v>
       </c>
       <c r="D105" t="s">
         <v>327</v>
@@ -5412,7 +5430,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="106" spans="1:11">
+    <row r="106" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>115</v>
       </c>
@@ -5420,7 +5438,7 @@
         <v>226</v>
       </c>
       <c r="C106" s="3">
-        <v>45314.67109953704</v>
+        <v>45314.671099537038</v>
       </c>
       <c r="D106" t="s">
         <v>328</v>
@@ -5444,7 +5462,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="107" spans="1:11">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>116</v>
       </c>
@@ -5452,7 +5470,7 @@
         <v>169</v>
       </c>
       <c r="C107" s="3">
-        <v>45314.69586805555</v>
+        <v>45314.695868055547</v>
       </c>
       <c r="D107" t="s">
         <v>272</v>
@@ -5473,7 +5491,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="108" spans="1:11">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>117</v>
       </c>
@@ -5481,7 +5499,7 @@
         <v>227</v>
       </c>
       <c r="C108" s="3">
-        <v>45315.49449074074</v>
+        <v>45315.494490740741</v>
       </c>
       <c r="D108" t="s">
         <v>329</v>
@@ -5505,7 +5523,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="109" spans="1:11">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>118</v>
       </c>
@@ -5513,7 +5531,7 @@
         <v>228</v>
       </c>
       <c r="C109" s="3">
-        <v>45315.54480324074</v>
+        <v>45315.544803240737</v>
       </c>
       <c r="D109" t="s">
         <v>330</v>
@@ -5537,7 +5555,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="110" spans="1:11">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>119</v>
       </c>
@@ -5545,7 +5563,7 @@
         <v>191</v>
       </c>
       <c r="C110" s="3">
-        <v>45315.62829861111</v>
+        <v>45315.628298611111</v>
       </c>
       <c r="D110" t="s">
         <v>295</v>
@@ -5566,7 +5584,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="111" spans="1:11">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>120</v>
       </c>
@@ -5574,7 +5592,7 @@
         <v>229</v>
       </c>
       <c r="C111" s="3">
-        <v>45315.7253125</v>
+        <v>45315.725312499999</v>
       </c>
       <c r="D111" t="s">
         <v>331</v>
@@ -5598,7 +5616,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="112" spans="1:11">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>121</v>
       </c>
@@ -5606,7 +5624,7 @@
         <v>194</v>
       </c>
       <c r="C112" s="3">
-        <v>45316.40819444445</v>
+        <v>45316.408194444448</v>
       </c>
       <c r="D112" t="s">
         <v>298</v>
@@ -5630,7 +5648,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="113" spans="1:11">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>122</v>
       </c>
@@ -5638,7 +5656,7 @@
         <v>230</v>
       </c>
       <c r="C113" s="3">
-        <v>45316.55929398148</v>
+        <v>45316.559293981481</v>
       </c>
       <c r="D113" t="s">
         <v>332</v>
@@ -5662,7 +5680,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="114" spans="1:11">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>123</v>
       </c>
@@ -5670,7 +5688,7 @@
         <v>231</v>
       </c>
       <c r="C114" s="3">
-        <v>45317.42777777778</v>
+        <v>45317.427777777782</v>
       </c>
       <c r="D114" t="s">
         <v>333</v>
@@ -5694,7 +5712,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="115" spans="1:11">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>124</v>
       </c>
@@ -5702,7 +5720,7 @@
         <v>231</v>
       </c>
       <c r="C115" s="3">
-        <v>45317.43003472222</v>
+        <v>45317.430034722223</v>
       </c>
       <c r="D115" t="s">
         <v>333</v>
@@ -5726,7 +5744,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="116" spans="1:11">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>125</v>
       </c>
@@ -5734,7 +5752,7 @@
         <v>232</v>
       </c>
       <c r="C116" s="3">
-        <v>45317.59055555556</v>
+        <v>45317.590555555558</v>
       </c>
       <c r="D116" t="s">
         <v>334</v>
@@ -5758,7 +5776,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="117" spans="1:11">
+    <row r="117" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>126</v>
       </c>
@@ -5766,7 +5784,7 @@
         <v>233</v>
       </c>
       <c r="C117" s="3">
-        <v>45317.75788194445</v>
+        <v>45317.757881944453</v>
       </c>
       <c r="D117" t="s">
         <v>335</v>
@@ -5790,7 +5808,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="118" spans="1:11">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>127</v>
       </c>
@@ -5798,7 +5816,7 @@
         <v>234</v>
       </c>
       <c r="C118" s="3">
-        <v>45318.4338425926</v>
+        <v>45318.433842592603</v>
       </c>
       <c r="D118" t="s">
         <v>336</v>
@@ -5822,7 +5840,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="119" spans="1:11">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>128</v>
       </c>
@@ -5830,7 +5848,7 @@
         <v>234</v>
       </c>
       <c r="C119" s="3">
-        <v>45318.43528935185</v>
+        <v>45318.435289351852</v>
       </c>
       <c r="D119" t="s">
         <v>336</v>
@@ -5854,7 +5872,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="120" spans="1:11">
+    <row r="120" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>129</v>
       </c>
@@ -5862,7 +5880,7 @@
         <v>235</v>
       </c>
       <c r="C120" s="3">
-        <v>45318.52028935185</v>
+        <v>45318.520289351851</v>
       </c>
       <c r="D120" t="s">
         <v>337</v>
@@ -5883,7 +5901,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="121" spans="1:11">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>130</v>
       </c>
@@ -5891,7 +5909,7 @@
         <v>236</v>
       </c>
       <c r="C121" s="3">
-        <v>45318.53774305555</v>
+        <v>45318.537743055553</v>
       </c>
       <c r="D121" t="s">
         <v>338</v>
@@ -5915,7 +5933,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="122" spans="1:11">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>131</v>
       </c>
@@ -5923,7 +5941,7 @@
         <v>231</v>
       </c>
       <c r="C122" s="3">
-        <v>45320.44130787037</v>
+        <v>45320.441307870373</v>
       </c>
       <c r="D122" t="s">
         <v>333</v>
@@ -5947,7 +5965,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="123" spans="1:11">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>132</v>
       </c>
@@ -5955,7 +5973,7 @@
         <v>237</v>
       </c>
       <c r="C123" s="3">
-        <v>45320.48193287037</v>
+        <v>45320.481932870367</v>
       </c>
       <c r="D123" t="s">
         <v>339</v>
@@ -5979,7 +5997,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="124" spans="1:11">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>133</v>
       </c>
@@ -5987,7 +6005,7 @@
         <v>237</v>
       </c>
       <c r="C124" s="3">
-        <v>45320.48549768519</v>
+        <v>45320.485497685193</v>
       </c>
       <c r="D124" t="s">
         <v>339</v>
@@ -6011,7 +6029,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="125" spans="1:11">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>134</v>
       </c>
@@ -6019,7 +6037,7 @@
         <v>237</v>
       </c>
       <c r="C125" s="3">
-        <v>45320.4875</v>
+        <v>45320.487500000003</v>
       </c>
       <c r="D125" t="s">
         <v>339</v>
@@ -6043,7 +6061,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="126" spans="1:11">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>135</v>
       </c>
@@ -6075,7 +6093,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="127" spans="1:11">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>136</v>
       </c>
@@ -6083,7 +6101,7 @@
         <v>239</v>
       </c>
       <c r="C127" s="3">
-        <v>45320.52901620371</v>
+        <v>45320.529016203713</v>
       </c>
       <c r="D127" t="s">
         <v>341</v>
@@ -6107,7 +6125,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="128" spans="1:11">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>137</v>
       </c>
@@ -6115,7 +6133,7 @@
         <v>240</v>
       </c>
       <c r="C128" s="3">
-        <v>45320.57282407407</v>
+        <v>45320.572824074072</v>
       </c>
       <c r="D128" t="s">
         <v>342</v>
@@ -6136,7 +6154,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="129" spans="1:11">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>138</v>
       </c>
@@ -6144,7 +6162,7 @@
         <v>241</v>
       </c>
       <c r="C129" s="3">
-        <v>45320.61900462963</v>
+        <v>45320.619004629632</v>
       </c>
       <c r="D129" t="s">
         <v>288</v>
@@ -6168,7 +6186,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="130" spans="1:11">
+    <row r="130" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>139</v>
       </c>
@@ -6176,7 +6194,7 @@
         <v>242</v>
       </c>
       <c r="C130" s="3">
-        <v>45321.38232638889</v>
+        <v>45321.382326388892</v>
       </c>
       <c r="D130" t="s">
         <v>343</v>
@@ -6200,7 +6218,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="131" spans="1:11">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>140</v>
       </c>
@@ -6229,7 +6247,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="132" spans="1:11">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>141</v>
       </c>
@@ -6237,7 +6255,7 @@
         <v>244</v>
       </c>
       <c r="C132" s="3">
-        <v>45321.49140046296</v>
+        <v>45321.491400462961</v>
       </c>
       <c r="D132" t="s">
         <v>288</v>
@@ -6261,7 +6279,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="133" spans="1:11">
+    <row r="133" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>142</v>
       </c>
@@ -6269,7 +6287,7 @@
         <v>245</v>
       </c>
       <c r="C133" s="3">
-        <v>45322.39694444444</v>
+        <v>45322.396944444437</v>
       </c>
       <c r="D133" t="s">
         <v>344</v>
@@ -6293,7 +6311,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="134" spans="1:11">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>143</v>
       </c>
@@ -6301,7 +6319,7 @@
         <v>246</v>
       </c>
       <c r="C134" s="3">
-        <v>45322.71115740741</v>
+        <v>45322.711157407408</v>
       </c>
       <c r="D134" t="s">
         <v>288</v>
@@ -6320,6 +6338,20 @@
       </c>
       <c r="K134" t="s">
         <v>540</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F135">
+        <f>SUM(F2:F134)</f>
+        <v>50458.549999999996</v>
+      </c>
+      <c r="G135">
+        <f>SUM(G2:G134)</f>
+        <v>123900.8</v>
+      </c>
+      <c r="H135">
+        <f>G135-F135</f>
+        <v>73442.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>